<commit_message>
Minor update to Restoration_Prioritization_Output_for_WebMap_Table
</commit_message>
<xml_diff>
--- a/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
@@ -360,22 +360,22 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>ReachName</t>
+          <t>Reach Name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>RM_Start</t>
+          <t>River Mile - Start</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RM_End</t>
+          <t>River Mile - End</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Assessment.Unit</t>
+          <t>Assessment Unit</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -385,12 +385,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Life_Stages</t>
+          <t>Life Stages</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Limiting Factors</t>
+          <t>Limiting Factor</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
rounded river mile output to two decimal places
</commit_message>
<xml_diff>
--- a/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
@@ -409,7 +409,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.659388</v>
+        <v>0.66</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -444,10 +444,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>11.8521</v>
+        <v>11.85</v>
       </c>
       <c r="C3">
-        <v>13.3869</v>
+        <v>13.39</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -482,10 +482,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>13.3869</v>
+        <v>13.39</v>
       </c>
       <c r="C4">
-        <v>14.3991</v>
+        <v>14.4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -520,10 +520,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>14.3991</v>
+        <v>14.4</v>
       </c>
       <c r="C5">
-        <v>14.7674</v>
+        <v>14.77</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -558,10 +558,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>14.7674</v>
+        <v>14.77</v>
       </c>
       <c r="C6">
-        <v>16.1895</v>
+        <v>16.19</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>16.1895</v>
+        <v>16.19</v>
       </c>
       <c r="C7">
-        <v>18.447</v>
+        <v>18.45</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -634,10 +634,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>18.447</v>
+        <v>18.45</v>
       </c>
       <c r="C8">
-        <v>20.3407</v>
+        <v>20.34</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -672,10 +672,10 @@
         </is>
       </c>
       <c r="B9">
-        <v>20.3407</v>
+        <v>20.34</v>
       </c>
       <c r="C9">
-        <v>21.1877</v>
+        <v>21.19</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -710,10 +710,10 @@
         </is>
       </c>
       <c r="B10">
-        <v>21.1877</v>
+        <v>21.19</v>
       </c>
       <c r="C10">
-        <v>23.3224</v>
+        <v>23.32</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -748,10 +748,10 @@
         </is>
       </c>
       <c r="B11">
-        <v>23.3224</v>
+        <v>23.32</v>
       </c>
       <c r="C11">
-        <v>24.2879</v>
+        <v>24.29</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>1.1389</v>
+        <v>1.14</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -824,10 +824,10 @@
         </is>
       </c>
       <c r="B13">
-        <v>1.1389</v>
+        <v>1.14</v>
       </c>
       <c r="C13">
-        <v>2.33753</v>
+        <v>2.34</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -862,10 +862,10 @@
         </is>
       </c>
       <c r="B14">
-        <v>2.33753</v>
+        <v>2.34</v>
       </c>
       <c r="C14">
-        <v>4.06948</v>
+        <v>4.07</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -900,10 +900,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>4.06948</v>
+        <v>4.07</v>
       </c>
       <c r="C15">
-        <v>5.73668</v>
+        <v>5.74</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -938,10 +938,10 @@
         </is>
       </c>
       <c r="B16">
-        <v>5.73668</v>
+        <v>5.74</v>
       </c>
       <c r="C16">
-        <v>7.05892</v>
+        <v>7.06</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -976,10 +976,10 @@
         </is>
       </c>
       <c r="B17">
-        <v>7.05892</v>
+        <v>7.06</v>
       </c>
       <c r="C17">
-        <v>7.43586</v>
+        <v>7.44</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1014,10 +1014,10 @@
         </is>
       </c>
       <c r="B18">
-        <v>7.43586</v>
+        <v>7.44</v>
       </c>
       <c r="C18">
-        <v>8.635109999999999</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1052,10 +1052,10 @@
         </is>
       </c>
       <c r="B19">
-        <v>8.635109999999999</v>
+        <v>8.640000000000001</v>
       </c>
       <c r="C19">
-        <v>9.50724</v>
+        <v>9.51</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1090,10 +1090,10 @@
         </is>
       </c>
       <c r="B20">
-        <v>9.50724</v>
+        <v>9.51</v>
       </c>
       <c r="C20">
-        <v>9.971120000000001</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1128,10 +1128,10 @@
         </is>
       </c>
       <c r="B21">
-        <v>9.971120000000001</v>
+        <v>9.970000000000001</v>
       </c>
       <c r="C21">
-        <v>10.6495</v>
+        <v>10.65</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1166,10 +1166,10 @@
         </is>
       </c>
       <c r="B22">
-        <v>10.6495</v>
+        <v>10.65</v>
       </c>
       <c r="C22">
-        <v>11.8521</v>
+        <v>11.85</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1204,10 +1204,10 @@
         </is>
       </c>
       <c r="B23">
-        <v>24.2879</v>
+        <v>24.29</v>
       </c>
       <c r="C23">
-        <v>25.6372</v>
+        <v>25.64</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1242,10 +1242,10 @@
         </is>
       </c>
       <c r="B24">
-        <v>25.6372</v>
+        <v>25.64</v>
       </c>
       <c r="C24">
-        <v>27.0652</v>
+        <v>27.07</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>1.89492</v>
+        <v>1.89</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1318,10 +1318,10 @@
         </is>
       </c>
       <c r="B26">
-        <v>1.89492</v>
+        <v>1.89</v>
       </c>
       <c r="C26">
-        <v>2.92462</v>
+        <v>2.92</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1356,10 +1356,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>2.92462</v>
+        <v>2.92</v>
       </c>
       <c r="C27">
-        <v>5.46548</v>
+        <v>5.47</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1394,10 +1394,10 @@
         </is>
       </c>
       <c r="B28">
-        <v>5.46548</v>
+        <v>5.47</v>
       </c>
       <c r="C28">
-        <v>7.14957</v>
+        <v>7.15</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1432,10 +1432,10 @@
         </is>
       </c>
       <c r="B29">
-        <v>7.14957</v>
+        <v>7.15</v>
       </c>
       <c r="C29">
-        <v>9.53525</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1470,10 +1470,10 @@
         </is>
       </c>
       <c r="B30">
-        <v>9.53525</v>
+        <v>9.539999999999999</v>
       </c>
       <c r="C30">
-        <v>11.1735</v>
+        <v>11.17</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1508,10 +1508,10 @@
         </is>
       </c>
       <c r="B31">
-        <v>11.1735</v>
+        <v>11.17</v>
       </c>
       <c r="C31">
-        <v>13.101</v>
+        <v>13.1</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1546,10 +1546,10 @@
         </is>
       </c>
       <c r="B32">
-        <v>27.0223</v>
+        <v>27.02</v>
       </c>
       <c r="C32">
-        <v>27.469</v>
+        <v>27.47</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1584,10 +1584,10 @@
         </is>
       </c>
       <c r="B33">
-        <v>27.469</v>
+        <v>27.47</v>
       </c>
       <c r="C33">
-        <v>28.2527</v>
+        <v>28.25</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1622,10 +1622,10 @@
         </is>
       </c>
       <c r="B34">
-        <v>28.6932</v>
+        <v>28.69</v>
       </c>
       <c r="C34">
-        <v>29.2987</v>
+        <v>29.3</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1660,10 +1660,10 @@
         </is>
       </c>
       <c r="B35">
-        <v>31.0893</v>
+        <v>31.09</v>
       </c>
       <c r="C35">
-        <v>31.5953</v>
+        <v>31.6</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1698,10 +1698,10 @@
         </is>
       </c>
       <c r="B36">
-        <v>31.5953</v>
+        <v>31.6</v>
       </c>
       <c r="C36">
-        <v>32.0922</v>
+        <v>32.09</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1736,10 +1736,10 @@
         </is>
       </c>
       <c r="B37">
-        <v>32.3712</v>
+        <v>32.37</v>
       </c>
       <c r="C37">
-        <v>33.1816</v>
+        <v>33.18</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1774,10 +1774,10 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.507941</v>
+        <v>0.51</v>
       </c>
       <c r="C38">
-        <v>1.30165</v>
+        <v>1.3</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1812,10 +1812,10 @@
         </is>
       </c>
       <c r="B39">
-        <v>1.30165</v>
+        <v>1.3</v>
       </c>
       <c r="C39">
-        <v>3.36657</v>
+        <v>3.37</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1850,10 +1850,10 @@
         </is>
       </c>
       <c r="B40">
-        <v>3.36657</v>
+        <v>3.37</v>
       </c>
       <c r="C40">
-        <v>4.01284</v>
+        <v>4.01</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1888,10 +1888,10 @@
         </is>
       </c>
       <c r="B41">
-        <v>4.01284</v>
+        <v>4.01</v>
       </c>
       <c r="C41">
-        <v>5.79279</v>
+        <v>5.79</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1926,10 +1926,10 @@
         </is>
       </c>
       <c r="B42">
-        <v>5.79279</v>
+        <v>5.79</v>
       </c>
       <c r="C42">
-        <v>6.59941</v>
+        <v>6.6</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1964,10 +1964,10 @@
         </is>
       </c>
       <c r="B43">
-        <v>16.2977</v>
+        <v>16.3</v>
       </c>
       <c r="C43">
-        <v>18.7001</v>
+        <v>18.7</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2002,10 +2002,10 @@
         </is>
       </c>
       <c r="B44">
-        <v>18.7001</v>
+        <v>18.7</v>
       </c>
       <c r="C44">
-        <v>20.5033</v>
+        <v>20.5</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -2040,10 +2040,10 @@
         </is>
       </c>
       <c r="B45">
-        <v>20.5033</v>
+        <v>20.5</v>
       </c>
       <c r="C45">
-        <v>21.8268</v>
+        <v>21.83</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -2078,10 +2078,10 @@
         </is>
       </c>
       <c r="B46">
-        <v>21.8268</v>
+        <v>21.83</v>
       </c>
       <c r="C46">
-        <v>22.1291</v>
+        <v>22.13</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2116,10 +2116,10 @@
         </is>
       </c>
       <c r="B47">
-        <v>22.1291</v>
+        <v>22.13</v>
       </c>
       <c r="C47">
-        <v>23.8768</v>
+        <v>23.88</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -2154,10 +2154,10 @@
         </is>
       </c>
       <c r="B48">
-        <v>23.8768</v>
+        <v>23.88</v>
       </c>
       <c r="C48">
-        <v>24.5381</v>
+        <v>24.54</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -2192,10 +2192,10 @@
         </is>
       </c>
       <c r="B49">
-        <v>24.5381</v>
+        <v>24.54</v>
       </c>
       <c r="C49">
-        <v>25.2848</v>
+        <v>25.28</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -2230,10 +2230,10 @@
         </is>
       </c>
       <c r="B50">
-        <v>25.2848</v>
+        <v>25.28</v>
       </c>
       <c r="C50">
-        <v>26.3748</v>
+        <v>26.37</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -2268,10 +2268,10 @@
         </is>
       </c>
       <c r="B51">
-        <v>26.3748</v>
+        <v>26.37</v>
       </c>
       <c r="C51">
-        <v>27.0223</v>
+        <v>27.02</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -2306,10 +2306,10 @@
         </is>
       </c>
       <c r="B52">
-        <v>3.7277</v>
+        <v>3.73</v>
       </c>
       <c r="C52">
-        <v>4.51119</v>
+        <v>4.51</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <v>0.8270650000000001</v>
+        <v>0.83</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -2382,10 +2382,10 @@
         </is>
       </c>
       <c r="B54">
-        <v>0.8270650000000001</v>
+        <v>0.83</v>
       </c>
       <c r="C54">
-        <v>1.90929</v>
+        <v>1.91</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -2420,10 +2420,10 @@
         </is>
       </c>
       <c r="B55">
-        <v>2.59519</v>
+        <v>2.6</v>
       </c>
       <c r="C55">
-        <v>4.93638</v>
+        <v>4.94</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -2458,10 +2458,10 @@
         </is>
       </c>
       <c r="B56">
-        <v>4.93638</v>
+        <v>4.94</v>
       </c>
       <c r="C56">
-        <v>6.69039</v>
+        <v>6.69</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -2496,10 +2496,10 @@
         </is>
       </c>
       <c r="B57">
-        <v>6.69039</v>
+        <v>6.69</v>
       </c>
       <c r="C57">
-        <v>7.84324</v>
+        <v>7.84</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -2534,10 +2534,10 @@
         </is>
       </c>
       <c r="B58">
-        <v>54.4957</v>
+        <v>54.5</v>
       </c>
       <c r="C58">
-        <v>55.4061</v>
+        <v>55.41</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -2572,10 +2572,10 @@
         </is>
       </c>
       <c r="B59">
-        <v>55.4061</v>
+        <v>55.41</v>
       </c>
       <c r="C59">
-        <v>56.9966</v>
+        <v>57</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -2610,10 +2610,10 @@
         </is>
       </c>
       <c r="B60">
-        <v>56.9966</v>
+        <v>57</v>
       </c>
       <c r="C60">
-        <v>59.3551</v>
+        <v>59.36</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2648,10 +2648,10 @@
         </is>
       </c>
       <c r="B61">
-        <v>60.5529</v>
+        <v>60.55</v>
       </c>
       <c r="C61">
-        <v>61.6703</v>
+        <v>61.67</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -2686,10 +2686,10 @@
         </is>
       </c>
       <c r="B62">
-        <v>61.6703</v>
+        <v>61.67</v>
       </c>
       <c r="C62">
-        <v>62.2979</v>
+        <v>62.3</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -2724,10 +2724,10 @@
         </is>
       </c>
       <c r="B63">
-        <v>62.2979</v>
+        <v>62.3</v>
       </c>
       <c r="C63">
-        <v>63.5317</v>
+        <v>63.53</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2762,10 +2762,10 @@
         </is>
       </c>
       <c r="B64">
-        <v>63.5317</v>
+        <v>63.53</v>
       </c>
       <c r="C64">
-        <v>66.0474</v>
+        <v>66.05</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2800,10 +2800,10 @@
         </is>
       </c>
       <c r="B65">
-        <v>66.0474</v>
+        <v>66.05</v>
       </c>
       <c r="C65">
-        <v>66.8323</v>
+        <v>66.83</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -2838,10 +2838,10 @@
         </is>
       </c>
       <c r="B66">
-        <v>66.8323</v>
+        <v>66.83</v>
       </c>
       <c r="C66">
-        <v>67.9504</v>
+        <v>67.95</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -2876,10 +2876,10 @@
         </is>
       </c>
       <c r="B67">
-        <v>67.9504</v>
+        <v>67.95</v>
       </c>
       <c r="C67">
-        <v>69.9508</v>
+        <v>69.95</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -2914,10 +2914,10 @@
         </is>
       </c>
       <c r="B68">
-        <v>11.4693</v>
+        <v>11.47</v>
       </c>
       <c r="C68">
-        <v>13.943</v>
+        <v>13.94</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -2952,10 +2952,10 @@
         </is>
       </c>
       <c r="B69">
-        <v>17.7471</v>
+        <v>17.75</v>
       </c>
       <c r="C69">
-        <v>19.8888</v>
+        <v>19.89</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2990,10 +2990,10 @@
         </is>
       </c>
       <c r="B70">
-        <v>19.8888</v>
+        <v>19.89</v>
       </c>
       <c r="C70">
-        <v>21.5552</v>
+        <v>21.56</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -3028,10 +3028,10 @@
         </is>
       </c>
       <c r="B71">
-        <v>69.9508</v>
+        <v>69.95</v>
       </c>
       <c r="C71">
-        <v>72.2741</v>
+        <v>72.27</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -3066,10 +3066,10 @@
         </is>
       </c>
       <c r="B72">
-        <v>72.2741</v>
+        <v>72.27</v>
       </c>
       <c r="C72">
-        <v>74.017</v>
+        <v>74.02</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -3104,10 +3104,10 @@
         </is>
       </c>
       <c r="B73">
-        <v>74.017</v>
+        <v>74.02</v>
       </c>
       <c r="C73">
-        <v>75.93850000000001</v>
+        <v>75.94</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -3142,10 +3142,10 @@
         </is>
       </c>
       <c r="B74">
-        <v>75.93850000000001</v>
+        <v>75.94</v>
       </c>
       <c r="C74">
-        <v>77.54470000000001</v>
+        <v>77.54000000000001</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -3180,10 +3180,10 @@
         </is>
       </c>
       <c r="B75">
-        <v>77.54470000000001</v>
+        <v>77.54000000000001</v>
       </c>
       <c r="C75">
-        <v>79.29989999999999</v>
+        <v>79.3</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -3221,7 +3221,7 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>0.745062</v>
+        <v>0.75</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -3256,10 +3256,10 @@
         </is>
       </c>
       <c r="B77">
-        <v>0.745062</v>
+        <v>0.75</v>
       </c>
       <c r="C77">
-        <v>1.49499</v>
+        <v>1.49</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -3294,10 +3294,10 @@
         </is>
       </c>
       <c r="B78">
-        <v>1.13489</v>
+        <v>1.13</v>
       </c>
       <c r="C78">
-        <v>2.49619</v>
+        <v>2.5</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -3332,10 +3332,10 @@
         </is>
       </c>
       <c r="B79">
-        <v>4.98959</v>
+        <v>4.99</v>
       </c>
       <c r="C79">
-        <v>6.39975</v>
+        <v>6.4</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -3370,10 +3370,10 @@
         </is>
       </c>
       <c r="B80">
-        <v>6.39975</v>
+        <v>6.4</v>
       </c>
       <c r="C80">
-        <v>7.5062</v>
+        <v>7.51</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -3408,10 +3408,10 @@
         </is>
       </c>
       <c r="B81">
-        <v>7.5062</v>
+        <v>7.51</v>
       </c>
       <c r="C81">
-        <v>8.75653</v>
+        <v>8.76</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -3446,10 +3446,10 @@
         </is>
       </c>
       <c r="B82">
-        <v>8.75653</v>
+        <v>8.76</v>
       </c>
       <c r="C82">
-        <v>9.213150000000001</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -3484,10 +3484,10 @@
         </is>
       </c>
       <c r="B83">
-        <v>9.213150000000001</v>
+        <v>9.210000000000001</v>
       </c>
       <c r="C83">
-        <v>10.3616</v>
+        <v>10.36</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -3522,10 +3522,10 @@
         </is>
       </c>
       <c r="B84">
-        <v>10.3616</v>
+        <v>10.36</v>
       </c>
       <c r="C84">
-        <v>11.2025</v>
+        <v>11.2</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -3563,7 +3563,7 @@
         <v>12.02</v>
       </c>
       <c r="C85">
-        <v>12.6533</v>
+        <v>12.65</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         </is>
       </c>
       <c r="B86">
-        <v>12.6533</v>
+        <v>12.65</v>
       </c>
       <c r="C86">
-        <v>13.6217</v>
+        <v>13.62</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -3636,10 +3636,10 @@
         </is>
       </c>
       <c r="B87">
-        <v>13.6217</v>
+        <v>13.62</v>
       </c>
       <c r="C87">
-        <v>14.9302</v>
+        <v>14.93</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -3674,10 +3674,10 @@
         </is>
       </c>
       <c r="B88">
-        <v>14.9302</v>
+        <v>14.93</v>
       </c>
       <c r="C88">
-        <v>15.9266</v>
+        <v>15.93</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -3715,7 +3715,7 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>0.682389</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -3750,10 +3750,10 @@
         </is>
       </c>
       <c r="B90">
-        <v>0.682389</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="C90">
-        <v>1.69161</v>
+        <v>1.69</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -3788,10 +3788,10 @@
         </is>
       </c>
       <c r="B91">
-        <v>1.69161</v>
+        <v>1.69</v>
       </c>
       <c r="C91">
-        <v>2.81973</v>
+        <v>2.82</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -3826,10 +3826,10 @@
         </is>
       </c>
       <c r="B92">
-        <v>2.81973</v>
+        <v>2.82</v>
       </c>
       <c r="C92">
-        <v>4.37545</v>
+        <v>4.38</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -3864,10 +3864,10 @@
         </is>
       </c>
       <c r="B93">
-        <v>4.37545</v>
+        <v>4.38</v>
       </c>
       <c r="C93">
-        <v>4.96852</v>
+        <v>4.97</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -3902,10 +3902,10 @@
         </is>
       </c>
       <c r="B94">
-        <v>4.96852</v>
+        <v>4.97</v>
       </c>
       <c r="C94">
-        <v>6.62346</v>
+        <v>6.62</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -3940,10 +3940,10 @@
         </is>
       </c>
       <c r="B95">
-        <v>6.62346</v>
+        <v>6.62</v>
       </c>
       <c r="C95">
-        <v>7.71025</v>
+        <v>7.71</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -3978,10 +3978,10 @@
         </is>
       </c>
       <c r="B96">
-        <v>7.71025</v>
+        <v>7.71</v>
       </c>
       <c r="C96">
-        <v>9.03523</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -4016,10 +4016,10 @@
         </is>
       </c>
       <c r="B97">
-        <v>9.03523</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="C97">
-        <v>9.624219999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -4054,10 +4054,10 @@
         </is>
       </c>
       <c r="B98">
-        <v>9.624219999999999</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="C98">
-        <v>11.9348</v>
+        <v>11.93</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -4092,10 +4092,10 @@
         </is>
       </c>
       <c r="B99">
-        <v>11.9348</v>
+        <v>11.93</v>
       </c>
       <c r="C99">
-        <v>13.2685</v>
+        <v>13.27</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -4130,10 +4130,10 @@
         </is>
       </c>
       <c r="B100">
-        <v>13.2685</v>
+        <v>13.27</v>
       </c>
       <c r="C100">
-        <v>14.2984</v>
+        <v>14.3</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -4168,10 +4168,10 @@
         </is>
       </c>
       <c r="B101">
-        <v>14.2984</v>
+        <v>14.3</v>
       </c>
       <c r="C101">
-        <v>15.8551</v>
+        <v>15.86</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -4206,10 +4206,10 @@
         </is>
       </c>
       <c r="B102">
-        <v>15.8551</v>
+        <v>15.86</v>
       </c>
       <c r="C102">
-        <v>16.7546</v>
+        <v>16.75</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -4244,10 +4244,10 @@
         </is>
       </c>
       <c r="B103">
-        <v>16.7546</v>
+        <v>16.75</v>
       </c>
       <c r="C103">
-        <v>17.045</v>
+        <v>17.05</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -4282,10 +4282,10 @@
         </is>
       </c>
       <c r="B104">
-        <v>17.045</v>
+        <v>17.05</v>
       </c>
       <c r="C104">
-        <v>17.8823</v>
+        <v>17.88</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -4320,10 +4320,10 @@
         </is>
       </c>
       <c r="B105">
-        <v>19.8407</v>
+        <v>19.84</v>
       </c>
       <c r="C105">
-        <v>20.9447</v>
+        <v>20.94</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -4358,10 +4358,10 @@
         </is>
       </c>
       <c r="B106">
-        <v>20.9447</v>
+        <v>20.94</v>
       </c>
       <c r="C106">
-        <v>21.6862</v>
+        <v>21.69</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -4396,10 +4396,10 @@
         </is>
       </c>
       <c r="B107">
-        <v>38.3999</v>
+        <v>38.4</v>
       </c>
       <c r="C107">
-        <v>40.5561</v>
+        <v>40.56</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -4434,10 +4434,10 @@
         </is>
       </c>
       <c r="B108">
-        <v>40.5561</v>
+        <v>40.56</v>
       </c>
       <c r="C108">
-        <v>41.7027</v>
+        <v>41.7</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -4472,10 +4472,10 @@
         </is>
       </c>
       <c r="B109">
-        <v>41.7027</v>
+        <v>41.7</v>
       </c>
       <c r="C109">
-        <v>42.9198</v>
+        <v>42.92</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -4510,10 +4510,10 @@
         </is>
       </c>
       <c r="B110">
-        <v>42.9198</v>
+        <v>42.92</v>
       </c>
       <c r="C110">
-        <v>44.623</v>
+        <v>44.62</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
@@ -4548,10 +4548,10 @@
         </is>
       </c>
       <c r="B111">
-        <v>44.623</v>
+        <v>44.62</v>
       </c>
       <c r="C111">
-        <v>46.088</v>
+        <v>46.09</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -4586,10 +4586,10 @@
         </is>
       </c>
       <c r="B112">
-        <v>46.088</v>
+        <v>46.09</v>
       </c>
       <c r="C112">
-        <v>47.5819</v>
+        <v>47.58</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
@@ -4624,10 +4624,10 @@
         </is>
       </c>
       <c r="B113">
-        <v>47.5819</v>
+        <v>47.58</v>
       </c>
       <c r="C113">
-        <v>48.1247</v>
+        <v>48.12</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
@@ -4662,10 +4662,10 @@
         </is>
       </c>
       <c r="B114">
-        <v>48.1247</v>
+        <v>48.12</v>
       </c>
       <c r="C114">
-        <v>49.3908</v>
+        <v>49.39</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -4700,10 +4700,10 @@
         </is>
       </c>
       <c r="B115">
-        <v>49.3908</v>
+        <v>49.39</v>
       </c>
       <c r="C115">
-        <v>51.3757</v>
+        <v>51.38</v>
       </c>
       <c r="D115" t="inlineStr">
         <is>
@@ -4738,10 +4738,10 @@
         </is>
       </c>
       <c r="B116">
-        <v>51.3757</v>
+        <v>51.38</v>
       </c>
       <c r="C116">
-        <v>53.5608</v>
+        <v>53.56</v>
       </c>
       <c r="D116" t="inlineStr">
         <is>
@@ -4776,10 +4776,10 @@
         </is>
       </c>
       <c r="B117">
-        <v>53.5608</v>
+        <v>53.56</v>
       </c>
       <c r="C117">
-        <v>54.0613</v>
+        <v>54.06</v>
       </c>
       <c r="D117" t="inlineStr">
         <is>
@@ -4814,10 +4814,10 @@
         </is>
       </c>
       <c r="B118">
-        <v>17.2674</v>
+        <v>17.27</v>
       </c>
       <c r="C118">
-        <v>18.5024</v>
+        <v>18.5</v>
       </c>
       <c r="D118" t="inlineStr">
         <is>
@@ -4852,10 +4852,10 @@
         </is>
       </c>
       <c r="B119">
-        <v>18.5024</v>
+        <v>18.5</v>
       </c>
       <c r="C119">
-        <v>19.5608</v>
+        <v>19.56</v>
       </c>
       <c r="D119" t="inlineStr">
         <is>
@@ -4890,10 +4890,10 @@
         </is>
       </c>
       <c r="B120">
-        <v>19.5608</v>
+        <v>19.56</v>
       </c>
       <c r="C120">
-        <v>21.3418</v>
+        <v>21.34</v>
       </c>
       <c r="D120" t="inlineStr">
         <is>
@@ -4928,10 +4928,10 @@
         </is>
       </c>
       <c r="B121">
-        <v>21.3418</v>
+        <v>21.34</v>
       </c>
       <c r="C121">
-        <v>23.1651</v>
+        <v>23.17</v>
       </c>
       <c r="D121" t="inlineStr">
         <is>
@@ -4966,10 +4966,10 @@
         </is>
       </c>
       <c r="B122">
-        <v>23.1651</v>
+        <v>23.17</v>
       </c>
       <c r="C122">
-        <v>24.0583</v>
+        <v>24.06</v>
       </c>
       <c r="D122" t="inlineStr">
         <is>
@@ -5004,10 +5004,10 @@
         </is>
       </c>
       <c r="B123">
-        <v>24.0583</v>
+        <v>24.06</v>
       </c>
       <c r="C123">
-        <v>25.2926</v>
+        <v>25.29</v>
       </c>
       <c r="D123" t="inlineStr">
         <is>
@@ -5042,10 +5042,10 @@
         </is>
       </c>
       <c r="B124">
-        <v>8.283849999999999</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="C124">
-        <v>10.3133</v>
+        <v>10.31</v>
       </c>
       <c r="D124" t="inlineStr">
         <is>
@@ -5080,10 +5080,10 @@
         </is>
       </c>
       <c r="B125">
-        <v>10.3133</v>
+        <v>10.31</v>
       </c>
       <c r="C125">
-        <v>12.6715</v>
+        <v>12.67</v>
       </c>
       <c r="D125" t="inlineStr">
         <is>
@@ -5118,10 +5118,10 @@
         </is>
       </c>
       <c r="B126">
-        <v>12.6715</v>
+        <v>12.67</v>
       </c>
       <c r="C126">
-        <v>15.2198</v>
+        <v>15.22</v>
       </c>
       <c r="D126" t="inlineStr">
         <is>
@@ -5156,10 +5156,10 @@
         </is>
       </c>
       <c r="B127">
-        <v>15.2198</v>
+        <v>15.22</v>
       </c>
       <c r="C127">
-        <v>17.2674</v>
+        <v>17.27</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -5194,10 +5194,10 @@
         </is>
       </c>
       <c r="B128">
-        <v>25.2926</v>
+        <v>25.29</v>
       </c>
       <c r="C128">
-        <v>26.4888</v>
+        <v>26.49</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
@@ -5232,10 +5232,10 @@
         </is>
       </c>
       <c r="B129">
-        <v>26.4888</v>
+        <v>26.49</v>
       </c>
       <c r="C129">
-        <v>28.0004</v>
+        <v>28</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update WebMap output to include general Action column in output
</commit_message>
<xml_diff>
--- a/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H125"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -385,15 +385,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Action</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Priority Life Stages</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Limiting Factor</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Action Categories</t>
         </is>
@@ -423,15 +428,20 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>Restore Fish Passage</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Summer Rearing,Winter Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Fish Passage Barriers</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Fish Passage Restoration</t>
         </is>
@@ -461,15 +471,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -499,15 +514,20 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -537,15 +557,20 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -575,15 +600,20 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -613,15 +643,20 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Bank Restoration,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -651,15 +686,20 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -689,15 +729,20 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Pool Quantity and Quality,Riparian</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement</t>
         </is>
@@ -727,15 +772,20 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Pool Quantity and Quality,Riparian,Cover- Undercut Banks,Pools-DeepPools,Temperature-AdultHolding</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -765,15 +815,20 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management</t>
         </is>
@@ -803,15 +858,20 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Off-Channel- Side-Channels,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Bank Restoration,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -841,15 +901,20 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Off-Channel- Side-Channels,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Bank Restoration,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -879,15 +944,20 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -917,15 +987,20 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -955,15 +1030,20 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -993,15 +1073,20 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -1031,15 +1116,20 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -1069,15 +1159,20 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Water Quality Improvement</t>
         </is>
@@ -1107,15 +1202,20 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -1145,15 +1245,20 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -1183,15 +1288,20 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -1221,15 +1331,20 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Flow- Summer Base Flow,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Instream Flow Enhancement,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -1259,15 +1374,20 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Flow- Summer Base Flow,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Instream Flow Enhancement,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -1297,15 +1417,20 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>PRCNT Fines and Embeddedness,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Cover- Undercut Banks,Food-FoodWebResources,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Enhance Food Resources,Water Quality Improvement</t>
         </is>
@@ -1335,15 +1460,20 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration</t>
         </is>
@@ -1373,15 +1503,20 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration</t>
         </is>
@@ -1411,15 +1546,20 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration</t>
         </is>
@@ -1449,15 +1589,20 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Cover- Undercut Banks,Food-FoodWebResources,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Enhance Food Resources,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -1487,15 +1632,20 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Food-FoodWebResources,Pool Quantity and Quality</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Enhance Food Resources,Fine Sediment Management</t>
         </is>
@@ -1525,15 +1675,20 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration</t>
         </is>
@@ -1563,15 +1718,20 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -1601,15 +1761,20 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>Summer Rearing,Adult Migration,Spawning and Incubation,Winter Rearing</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Water Quality Improvement</t>
         </is>
@@ -1639,15 +1804,20 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>Summer Rearing,Adult Migration,Spawning and Incubation,Winter Rearing</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -1677,15 +1847,20 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -1715,15 +1890,20 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
           <t>Fry,Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -1753,15 +1933,20 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement,Upland Management</t>
         </is>
@@ -1791,15 +1976,20 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -1829,15 +2019,20 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -1867,15 +2062,20 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement,Upland Management</t>
         </is>
@@ -1905,15 +2105,20 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>Adult Migration,Holding and Maturation,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="I41" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -1943,15 +2148,20 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>Cover- Boulders,Cover- Wood,Off-Channel- Side-Channels,Cover- Undercut Banks,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="I42" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -1981,15 +2191,20 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>Winter Rearing,Fry,Summer Rearing,BT Subadult Rearing,Adult Migration,Spawning and Incubation</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Temperature- Rearing,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="I43" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Water Quality Improvement</t>
         </is>
@@ -2019,15 +2234,20 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="H44" t="inlineStr">
         <is>
           <t>Stability,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="I44" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Instream Flow Enhancement,Upland Management,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -2057,15 +2277,20 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="H45" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="I45" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -2095,15 +2320,20 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="H46" t="inlineStr">
         <is>
           <t>Stability,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="I46" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Instream Flow Enhancement,Upland Management,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -2133,15 +2363,20 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="H47" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="I47" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -2171,15 +2406,20 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="H48" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
+      <c r="I48" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -2209,15 +2449,20 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
           <t>Winter Rearing,Adult Migration,Spawning and Incubation,Summer Rearing</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="H49" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Temperature- Rearing,Cover- Boulders</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
+      <c r="I49" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -2247,15 +2492,20 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
+          <t>Restore Fish Passage</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
           <t>Adult Migration,Holding,Spawning and Incubation,Fry Colonization,Summer Rearing,Winter Rearing,Smolt Outmigration,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="H50" t="inlineStr">
         <is>
           <t>Fish Passage Barriers</t>
         </is>
       </c>
-      <c r="H50" t="inlineStr">
+      <c r="I50" t="inlineStr">
         <is>
           <t>Fish Passage Restoration</t>
         </is>
@@ -2285,15 +2535,20 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
           <t>BT Subadult Rearing,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="H51" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
+      <c r="I51" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement</t>
         </is>
@@ -2323,15 +2578,20 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>Restore Fish Passage</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
           <t>Holding,Spawning and Incubation,Fry Colonization,Summer Rearing,Winter Rearing,Smolt Outmigration,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="H52" t="inlineStr">
         <is>
           <t>Fish Passage Barriers</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
+      <c r="I52" t="inlineStr">
         <is>
           <t>Fish Passage Restoration</t>
         </is>
@@ -2361,15 +2621,20 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="H53" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H53" t="inlineStr">
+      <c r="I53" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -2399,15 +2664,20 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="H54" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
+      <c r="I54" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -2437,15 +2707,20 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="H55" t="inlineStr">
         <is>
           <t>Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
+      <c r="I55" t="inlineStr">
         <is>
           <t>Channel Modification,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -2475,15 +2750,20 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="H56" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H56" t="inlineStr">
+      <c r="I56" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -2513,15 +2793,20 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
           <t>Fry,Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="H57" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H57" t="inlineStr">
+      <c r="I57" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -2551,15 +2836,20 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="H58" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr">
+      <c r="I58" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Water Quality Improvement</t>
         </is>
@@ -2589,15 +2879,20 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="H59" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
+      <c r="I59" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -2627,15 +2922,20 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="H60" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H60" t="inlineStr">
+      <c r="I60" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -2665,15 +2965,20 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="H61" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H61" t="inlineStr">
+      <c r="I61" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -2703,15 +3008,20 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="H62" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H62" t="inlineStr">
+      <c r="I62" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -2741,15 +3051,20 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G63" t="inlineStr">
+      <c r="H63" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H63" t="inlineStr">
+      <c r="I63" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -2779,15 +3094,20 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="H64" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H64" t="inlineStr">
+      <c r="I64" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -2817,15 +3137,20 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="H65" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
+      <c r="I65" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement</t>
         </is>
@@ -2855,15 +3180,20 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
           <t>Fry,Holding and Maturation,Spawning and Incubation,Winter Rearing</t>
         </is>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="H66" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian</t>
         </is>
       </c>
-      <c r="H66" t="inlineStr">
+      <c r="I66" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement</t>
         </is>
@@ -2893,15 +3223,20 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G67" t="inlineStr">
+      <c r="H67" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H67" t="inlineStr">
+      <c r="I67" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Water Quality Improvement</t>
         </is>
@@ -2931,15 +3266,20 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="H68" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="I68" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Water Quality Improvement</t>
         </is>
@@ -2969,15 +3309,20 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G69" t="inlineStr">
+      <c r="H69" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr">
+      <c r="I69" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -3007,15 +3352,20 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="H70" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H70" t="inlineStr">
+      <c r="I70" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -3045,15 +3395,20 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
           <t>Summer Rearing,Winter Rearing</t>
         </is>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="H71" t="inlineStr">
         <is>
           <t>Cover- Wood,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr">
+      <c r="I71" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3083,15 +3438,20 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
+          <t>Restore Fish Passage</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Fry,Winter Rearing,Smolt Outmigration</t>
         </is>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="H72" t="inlineStr">
         <is>
           <t>Fish Passage Barriers</t>
         </is>
       </c>
-      <c r="H72" t="inlineStr">
+      <c r="I72" t="inlineStr">
         <is>
           <t>Fish Passage Restoration</t>
         </is>
@@ -3121,15 +3481,20 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
+          <t>Restore Fish Passage</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Fry,Winter Rearing,Smolt Outmigration</t>
         </is>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="H73" t="inlineStr">
         <is>
           <t>Fish Passage Barriers</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
+      <c r="I73" t="inlineStr">
         <is>
           <t>Fish Passage Restoration</t>
         </is>
@@ -3159,15 +3524,20 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="H74" t="inlineStr">
         <is>
           <t>PRCNT Fines and Embeddedness,Off-Channel- Side-Channels,Temperature- Adult Spawning,Off-Channel- Floodplain,Brook Trout</t>
         </is>
       </c>
-      <c r="H74" t="inlineStr">
+      <c r="I74" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement,Floodplain Reconnection,Brook Trout Management</t>
         </is>
@@ -3197,15 +3567,20 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="H75" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Temperature- Adult Spawning,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H75" t="inlineStr">
+      <c r="I75" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3235,15 +3610,20 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G76" t="inlineStr">
+      <c r="H76" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H76" t="inlineStr">
+      <c r="I76" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3273,15 +3653,20 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G77" t="inlineStr">
+      <c r="H77" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Temperature- Adult Spawning,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H77" t="inlineStr">
+      <c r="I77" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3311,15 +3696,20 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="H78" t="inlineStr">
         <is>
           <t>Contaminants,Flow- Summer Base Flow,Off-Channel- Side-Channels,Temperature- Adult Spawning,Cover- Wood,Off-Channel- Floodplain,Brook Trout</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr">
+      <c r="I78" t="inlineStr">
         <is>
           <t>Water Quality Improvement,Channel Modification,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Channel Complexity Restoration,Riparian Restoration and Management,Floodplain Reconnection,Brook Trout Management</t>
         </is>
@@ -3349,15 +3739,20 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G79" t="inlineStr">
+      <c r="H79" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Contaminants,Temperature- Adult Spawning,Cover- Boulders,Cover- Undercut Banks,Brook Trout</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
+      <c r="I79" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement,Brook Trout Management</t>
         </is>
@@ -3387,15 +3782,20 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G80" t="inlineStr">
+      <c r="H80" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Boulders,Cover- Undercut Banks,Brook Trout</t>
         </is>
       </c>
-      <c r="H80" t="inlineStr">
+      <c r="I80" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement,Brook Trout Management</t>
         </is>
@@ -3425,15 +3825,20 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Fry,BT Natal Rearing,Adult Migration</t>
         </is>
       </c>
-      <c r="G81" t="inlineStr">
+      <c r="H81" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Undercut Banks,Brook Trout</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr">
+      <c r="I81" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement,Brook Trout Management</t>
         </is>
@@ -3463,15 +3868,20 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="H82" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Undercut Banks,Brook Trout</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr">
+      <c r="I82" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement,Brook Trout Management</t>
         </is>
@@ -3501,15 +3911,20 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Adult Migration,Fry</t>
         </is>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="H83" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Boulders,Cover- Undercut Banks,Brook Trout</t>
         </is>
       </c>
-      <c r="H83" t="inlineStr">
+      <c r="I83" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement,Brook Trout Management</t>
         </is>
@@ -3539,15 +3954,20 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G84" t="inlineStr">
+      <c r="H84" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Brook Trout</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr">
+      <c r="I84" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement,Brook Trout Management</t>
         </is>
@@ -3577,15 +3997,20 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G85" t="inlineStr">
+      <c r="H85" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr">
+      <c r="I85" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3615,15 +4040,20 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="H86" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
+      <c r="I86" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3653,15 +4083,20 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="H87" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H87" t="inlineStr">
+      <c r="I87" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3691,15 +4126,20 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Holding and Maturation,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="H88" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks,Pools-DeepPools,Temperature-AdultHolding</t>
         </is>
       </c>
-      <c r="H88" t="inlineStr">
+      <c r="I88" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3729,15 +4169,20 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="H89" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H89" t="inlineStr">
+      <c r="I89" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3767,15 +4212,20 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="H90" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H90" t="inlineStr">
+      <c r="I90" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -3805,15 +4255,20 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="H91" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Cover- Undercut Banks,Entrainment and Stranding</t>
         </is>
       </c>
-      <c r="H91" t="inlineStr">
+      <c r="I91" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement,Entrainment and Stranding Mitigation</t>
         </is>
@@ -3843,15 +4298,20 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Adult Migration,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="H92" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Flow- Summer Base Flow,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H92" t="inlineStr">
+      <c r="I92" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -3881,15 +4341,20 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="H93" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Off-Channel- Floodplain,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H93" t="inlineStr">
+      <c r="I93" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -3919,15 +4384,20 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="H94" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H94" t="inlineStr">
+      <c r="I94" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -3957,15 +4427,20 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="H95" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H95" t="inlineStr">
+      <c r="I95" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -3995,15 +4470,20 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
           <t>Adult Migration,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G96" t="inlineStr">
+      <c r="H96" t="inlineStr">
         <is>
           <t>Stability,Flow- Summer Base Flow,Off-Channel- Floodplain,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H96" t="inlineStr">
+      <c r="I96" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Instream Flow Enhancement,Upland Management,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -4033,15 +4513,20 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
           <t>Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="H97" t="inlineStr">
         <is>
           <t>Stability,Off-Channel- Floodplain,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H97" t="inlineStr">
+      <c r="I97" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Instream Flow Enhancement,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -4071,15 +4556,20 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="H98" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H98" t="inlineStr">
+      <c r="I98" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4109,15 +4599,20 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="H99" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H99" t="inlineStr">
+      <c r="I99" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4147,15 +4642,20 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="H100" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H100" t="inlineStr">
+      <c r="I100" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4185,15 +4685,20 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G101" t="inlineStr">
+      <c r="H101" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing,Cover- Undercut Banks,Pools-DeepPools</t>
         </is>
       </c>
-      <c r="H101" t="inlineStr">
+      <c r="I101" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -4223,15 +4728,20 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Summer Rearing,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G102" t="inlineStr">
+      <c r="H102" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H102" t="inlineStr">
+      <c r="I102" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -4261,15 +4771,20 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
           <t>Summer Rearing,Holding and Maturation,Spawning and Incubation,Winter Rearing,Fry</t>
         </is>
       </c>
-      <c r="G103" t="inlineStr">
+      <c r="H103" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks,Pools-DeepPools,Temperature-AdultHolding</t>
         </is>
       </c>
-      <c r="H103" t="inlineStr">
+      <c r="I103" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4299,15 +4814,20 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
           <t>Summer Rearing,Spawning and Incubation,Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G104" t="inlineStr">
+      <c r="H104" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H104" t="inlineStr">
+      <c r="I104" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4337,15 +4857,20 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="H105" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H105" t="inlineStr">
+      <c r="I105" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4375,15 +4900,20 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G106" t="inlineStr">
+      <c r="H106" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H106" t="inlineStr">
+      <c r="I106" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4413,15 +4943,20 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G107" t="inlineStr">
+      <c r="H107" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Cover- Undercut Banks,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H107" t="inlineStr">
+      <c r="I107" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -4451,15 +4986,20 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G108" t="inlineStr">
+      <c r="H108" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H108" t="inlineStr">
+      <c r="I108" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4489,15 +5029,20 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G109" t="inlineStr">
+      <c r="H109" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H109" t="inlineStr">
+      <c r="I109" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4527,15 +5072,20 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G110" t="inlineStr">
+      <c r="H110" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H110" t="inlineStr">
+      <c r="I110" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4565,15 +5115,20 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
           <t>Spawning and Incubation,Winter Rearing,Summer Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G111" t="inlineStr">
+      <c r="H111" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing,PRCNT Fines and Embeddedness,Temperature- Adult Spawning,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H111" t="inlineStr">
+      <c r="I111" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Water Quality Improvement</t>
         </is>
@@ -4603,15 +5158,20 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
           <t>Winter Rearing,Summer Rearing,Spawning and Incubation,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G112" t="inlineStr">
+      <c r="H112" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing,Cover- Boulders,Cover- Undercut Banks</t>
         </is>
       </c>
-      <c r="H112" t="inlineStr">
+      <c r="I112" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4641,15 +5201,20 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
           <t>Summer Rearing,Holding and Maturation,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G113" t="inlineStr">
+      <c r="H113" t="inlineStr">
         <is>
           <t>Cover- Undercut Banks,Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H113" t="inlineStr">
+      <c r="I113" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Modification,Riparian Restoration and Management,Channel Complexity Restoration,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Water Quality Improvement</t>
         </is>
@@ -4679,15 +5244,20 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
           <t>Winter Rearing,Adult Migration,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G114" t="inlineStr">
+      <c r="H114" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H114" t="inlineStr">
+      <c r="I114" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -4717,15 +5287,20 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G115" t="inlineStr">
+      <c r="H115" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H115" t="inlineStr">
+      <c r="I115" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4755,15 +5330,20 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
           <t>Winter Rearing,Adult Migration,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G116" t="inlineStr">
+      <c r="H116" t="inlineStr">
         <is>
           <t>Cover- Wood,Flow- Summer Base Flow,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H116" t="inlineStr">
+      <c r="I116" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Instream Flow Enhancement,Upland Management,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Floodplain Reconnection,Water Quality Improvement</t>
         </is>
@@ -4793,15 +5373,20 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
           <t>Winter Rearing,Adult Migration,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G117" t="inlineStr">
+      <c r="H117" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Flow- Summer Base Flow,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness</t>
         </is>
       </c>
-      <c r="H117" t="inlineStr">
+      <c r="I117" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Bank Restoration,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -4831,15 +5416,20 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Spawning and Incubation,Fry</t>
         </is>
       </c>
-      <c r="G118" t="inlineStr">
+      <c r="H118" t="inlineStr">
         <is>
           <t>Coarse Substrate,Cover- Wood,Pool Quantity and Quality,Riparian,Temperature- Rearing,PRCNT Fines and Embeddedness</t>
         </is>
       </c>
-      <c r="H118" t="inlineStr">
+      <c r="I118" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Bank Restoration,Floodplain Reconnection,Instream Flow Enhancement,Side Channel and Off-Channel Habitat Restoration,Water Quality Improvement</t>
         </is>
@@ -4869,15 +5459,20 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G119" t="inlineStr">
+      <c r="H119" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H119" t="inlineStr">
+      <c r="I119" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4907,15 +5502,20 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G120" t="inlineStr">
+      <c r="H120" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H120" t="inlineStr">
+      <c r="I120" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4945,15 +5545,20 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G121" t="inlineStr">
+      <c r="H121" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H121" t="inlineStr">
+      <c r="I121" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -4983,15 +5588,20 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G122" t="inlineStr">
+      <c r="H122" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H122" t="inlineStr">
+      <c r="I122" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -5021,15 +5631,20 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
           <t>Winter Rearing,Holding and Maturation,Fry</t>
         </is>
       </c>
-      <c r="G123" t="inlineStr">
+      <c r="H123" t="inlineStr">
         <is>
           <t>Stability,Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H123" t="inlineStr">
+      <c r="I123" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Riparian Restoration and Management,Fine Sediment Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -5059,15 +5674,20 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G124" t="inlineStr">
+      <c r="H124" t="inlineStr">
         <is>
           <t>Cover- Wood,Off-Channel- Floodplain,Off-Channel- Side-Channels,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H124" t="inlineStr">
+      <c r="I124" t="inlineStr">
         <is>
           <t>Channel Complexity Restoration,Channel Modification,Riparian Restoration and Management,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Bank Restoration,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>
@@ -5097,15 +5717,20 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
+          <t xml:space="preserve"> Restore Reach Function</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
           <t>Holding and Maturation,Spawning and Incubation,Fry,Winter Rearing</t>
         </is>
       </c>
-      <c r="G125" t="inlineStr">
+      <c r="H125" t="inlineStr">
         <is>
           <t>Stability,Coarse Substrate,Cover- Wood,Pool Quantity and Quality,Riparian,Temperature- Rearing</t>
         </is>
       </c>
-      <c r="H125" t="inlineStr">
+      <c r="I125" t="inlineStr">
         <is>
           <t>Bank Restoration,Channel Complexity Restoration,Channel Modification,Floodplain Reconnection,Side Channel and Off-Channel Habitat Restoration,Fine Sediment Management,Upland Management,Riparian Restoration and Management,Instream Flow Enhancement,Water Quality Improvement</t>
         </is>

</xml_diff>

<commit_message>
Minor update to Action column
</commit_message>
<xml_diff>
--- a/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
+++ b/Output/Restoration_Prioritization_Output_for_WebMap_Table.xlsx
@@ -471,7 +471,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -772,7 +772,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -858,7 +858,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -987,7 +987,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1030,7 +1030,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1417,7 +1417,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1460,7 +1460,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1546,7 +1546,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1589,7 +1589,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1632,7 +1632,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1804,7 +1804,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1847,7 +1847,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2105,7 +2105,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2148,7 +2148,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2191,7 +2191,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2234,7 +2234,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2277,7 +2277,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2406,7 +2406,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2535,7 +2535,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2664,7 +2664,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2707,7 +2707,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2750,7 +2750,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2793,7 +2793,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2879,7 +2879,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2922,7 +2922,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -3008,7 +3008,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
@@ -3094,7 +3094,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
@@ -3137,7 +3137,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3180,7 +3180,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -3223,7 +3223,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -3309,7 +3309,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3352,7 +3352,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -3395,7 +3395,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -3524,7 +3524,7 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
@@ -3567,7 +3567,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3739,7 +3739,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
@@ -3868,7 +3868,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3911,7 +3911,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3954,7 +3954,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3997,7 +3997,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -4040,7 +4040,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -4083,7 +4083,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -4126,7 +4126,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
@@ -4212,7 +4212,7 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
@@ -4255,7 +4255,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -4298,7 +4298,7 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
@@ -4384,7 +4384,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -4427,7 +4427,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -4470,7 +4470,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
@@ -4513,7 +4513,7 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -4599,7 +4599,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -4642,7 +4642,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -4685,7 +4685,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -4771,7 +4771,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G105" t="inlineStr">
@@ -4900,7 +4900,7 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -4986,7 +4986,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -5072,7 +5072,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -5115,7 +5115,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -5158,7 +5158,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -5201,7 +5201,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Address Limiting Factors</t>
+          <t>Address Limiting Factors</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -5244,7 +5244,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -5287,7 +5287,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -5330,7 +5330,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -5373,7 +5373,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -5416,7 +5416,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -5459,7 +5459,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -5502,7 +5502,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -5545,7 +5545,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G121" t="inlineStr">
@@ -5588,7 +5588,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -5631,7 +5631,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function, Address Limiting Factors</t>
+          <t>Restore Reach Function, Address Limiting Factors</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -5674,7 +5674,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -5717,7 +5717,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Restore Reach Function</t>
+          <t>Restore Reach Function</t>
         </is>
       </c>
       <c r="G125" t="inlineStr">

</xml_diff>